<commit_message>
changes with tableToJson script from Lars
</commit_message>
<xml_diff>
--- a/app/data/2016-01-14/format/ANDI_betaTemplate_0303.xlsx
+++ b/app/data/2016-01-14/format/ANDI_betaTemplate_0303.xlsx
@@ -50,7 +50,7 @@
     <t>Long name 2</t>
   </si>
   <si>
-    <t>long name 3</t>
+    <t>Long name 3</t>
   </si>
   <si>
     <t>SPSS name</t>
@@ -541,7 +541,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,8 +572,8 @@
   </sheetPr>
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -583,7 +583,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6153846153846"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.04858299595142"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.4412955465587"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4412955465587"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2186234817814"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="40.1133603238866"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.663967611336"/>

</xml_diff>